<commit_message>
added circle timer to commands, change item and command functions
</commit_message>
<xml_diff>
--- a/Ressources/Festival.xlsx
+++ b/Ressources/Festival.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Artiste base" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Classification" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Listes d'objets" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Complexification" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Musiques" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Artiste base'!$B$2:$E$91</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="291">
   <si>
     <t xml:space="preserve">Artistes</t>
   </si>
@@ -337,9 +338,6 @@
     <t xml:space="preserve">Kas:St</t>
   </si>
   <si>
-    <t xml:space="preserve">*</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kind of Guru</t>
   </si>
   <si>
@@ -899,6 +897,9 @@
   </si>
   <si>
     <t xml:space="preserve">Temps de lecture d'une demande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom de la musique</t>
   </si>
 </sst>
 </file>
@@ -988,7 +989,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1171,6 +1172,13 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1200,7 +1208,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1369,6 +1377,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1410,32 +1434,30 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFBFBFBF"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFA6A6A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAEAAAA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1459,16 +1481,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -1481,7 +1493,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF9C0006"/>
-      <rgbColor rgb="FF006100"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -1506,7 +1518,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00B0F0"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFC6EFCE"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFEB9C"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -1543,19 +1555,19 @@
     <tabColor rgb="FF757171"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E91"/>
+  <dimension ref="B2:E91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.73046875" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.75" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27"/>
   </cols>
   <sheetData>
@@ -2120,14 +2132,11 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="B42" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="C42" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>39</v>
@@ -2138,10 +2147,10 @@
     </row>
     <row r="43" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>39</v>
@@ -2152,10 +2161,10 @@
     </row>
     <row r="44" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>108</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>109</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>24</v>
@@ -2166,10 +2175,10 @@
     </row>
     <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>110</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>18</v>
@@ -2180,10 +2189,10 @@
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>18</v>
@@ -2194,7 +2203,7 @@
     </row>
     <row r="47" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>74</v>
@@ -2208,10 +2217,10 @@
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>115</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>116</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>18</v>
@@ -2222,10 +2231,10 @@
     </row>
     <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>117</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>118</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>10</v>
@@ -2236,24 +2245,24 @@
     </row>
     <row r="50" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>119</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>120</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>123</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>43</v>
@@ -2264,10 +2273,10 @@
     </row>
     <row r="52" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="D52" s="10" t="s">
         <v>36</v>
@@ -2278,10 +2287,10 @@
     </row>
     <row r="53" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="D53" s="10" t="s">
         <v>24</v>
@@ -2292,24 +2301,24 @@
     </row>
     <row r="54" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>129</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>131</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>132</v>
       </c>
       <c r="D55" s="10" t="s">
         <v>24</v>
@@ -2320,35 +2329,35 @@
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>133</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>134</v>
       </c>
       <c r="D56" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>136</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>137</v>
       </c>
       <c r="D57" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>64</v>
@@ -2357,15 +2366,15 @@
         <v>36</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>142</v>
       </c>
       <c r="D59" s="10" t="s">
         <v>39</v>
@@ -2376,10 +2385,10 @@
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>144</v>
       </c>
       <c r="D60" s="10" t="s">
         <v>18</v>
@@ -2390,21 +2399,21 @@
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>145</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>146</v>
       </c>
       <c r="D61" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>42</v>
@@ -2418,24 +2427,24 @@
     </row>
     <row r="63" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63" s="13" t="s">
         <v>149</v>
-      </c>
-      <c r="C63" s="13" t="s">
-        <v>150</v>
       </c>
       <c r="D63" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B64" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D64" s="10" t="s">
         <v>36</v>
@@ -2446,21 +2455,21 @@
     </row>
     <row r="65" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C65" s="9" t="s">
         <v>153</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>154</v>
       </c>
       <c r="D65" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>74</v>
@@ -2474,24 +2483,24 @@
     </row>
     <row r="67" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B67" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>157</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>158</v>
       </c>
       <c r="D67" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>161</v>
       </c>
       <c r="D68" s="10" t="s">
         <v>39</v>
@@ -2502,10 +2511,10 @@
     </row>
     <row r="69" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B69" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="D69" s="10" t="s">
         <v>10</v>
@@ -2516,24 +2525,24 @@
     </row>
     <row r="70" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B70" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="D70" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B71" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>167</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>168</v>
       </c>
       <c r="D71" s="10" t="s">
         <v>10</v>
@@ -2544,7 +2553,7 @@
     </row>
     <row r="72" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B72" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C72" s="9" t="s">
         <v>5</v>
@@ -2558,55 +2567,55 @@
     </row>
     <row r="73" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C73" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="D73" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="D73" s="10" t="s">
+      <c r="E73" s="11" t="s">
         <v>172</v>
-      </c>
-      <c r="E73" s="11" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B74" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C74" s="9" t="s">
         <v>174</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>175</v>
       </c>
       <c r="D74" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B75" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D75" s="10" t="s">
         <v>39</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E76" s="11" t="s">
         <v>46</v>
@@ -2614,24 +2623,24 @@
     </row>
     <row r="77" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C77" s="9" t="s">
         <v>180</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>181</v>
       </c>
       <c r="D77" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C78" s="9" t="s">
         <v>183</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>184</v>
       </c>
       <c r="D78" s="10" t="s">
         <v>36</v>
@@ -2642,24 +2651,24 @@
     </row>
     <row r="79" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B79" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>186</v>
       </c>
       <c r="D79" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B80" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>188</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>189</v>
       </c>
       <c r="D80" s="10" t="s">
         <v>36</v>
@@ -2670,10 +2679,10 @@
     </row>
     <row r="81" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B81" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>190</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>191</v>
       </c>
       <c r="D81" s="10" t="s">
         <v>6</v>
@@ -2684,7 +2693,7 @@
     </row>
     <row r="82" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>5</v>
@@ -2693,29 +2702,29 @@
         <v>6</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B83" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C83" s="9" t="s">
         <v>194</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>195</v>
       </c>
       <c r="D83" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B84" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C84" s="9" t="s">
         <v>197</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>198</v>
       </c>
       <c r="D84" s="10" t="s">
         <v>36</v>
@@ -2726,21 +2735,21 @@
     </row>
     <row r="85" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B85" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C85" s="9" t="s">
         <v>199</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>200</v>
       </c>
       <c r="D85" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B86" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C86" s="9" t="s">
         <v>42</v>
@@ -2754,10 +2763,10 @@
     </row>
     <row r="87" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B87" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C87" s="9" t="s">
         <v>203</v>
-      </c>
-      <c r="C87" s="9" t="s">
-        <v>204</v>
       </c>
       <c r="D87" s="10" t="s">
         <v>24</v>
@@ -2768,10 +2777,10 @@
     </row>
     <row r="88" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B88" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C88" s="9" t="s">
         <v>205</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>206</v>
       </c>
       <c r="D88" s="10" t="s">
         <v>18</v>
@@ -2782,10 +2791,10 @@
     </row>
     <row r="89" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B89" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C89" s="9" t="s">
         <v>207</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>208</v>
       </c>
       <c r="D89" s="10" t="s">
         <v>6</v>
@@ -2796,7 +2805,7 @@
     </row>
     <row r="90" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B90" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C90" s="9" t="s">
         <v>55</v>
@@ -2810,10 +2819,10 @@
     </row>
     <row r="91" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B91" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="C91" s="15" t="s">
         <v>210</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>211</v>
       </c>
       <c r="D91" s="16" t="s">
         <v>36</v>
@@ -2847,7 +2856,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.73046875" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.75" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.43"/>
@@ -2863,16 +2872,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>212</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>213</v>
       </c>
       <c r="G2" s="22" t="n">
         <v>1</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2892,7 +2901,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2912,7 +2921,7 @@
         <v>3</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2934,7 +2943,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D6" s="28" t="n">
         <v>4</v>
@@ -2958,7 +2967,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D8" s="28" t="n">
         <v>5</v>
@@ -3010,7 +3019,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D12" s="28" t="n">
         <v>7</v>
@@ -3024,7 +3033,7 @@
         <v>37</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D13" s="28" t="n">
         <v>8</v>
@@ -3038,7 +3047,7 @@
         <v>41</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D14" s="28" t="n">
         <v>9</v>
@@ -3052,7 +3061,7 @@
         <v>44</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D15" s="28" t="n">
         <v>9</v>
@@ -3066,7 +3075,7 @@
         <v>47</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D16" s="28" t="n">
         <v>7</v>
@@ -3080,7 +3089,7 @@
         <v>49</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D17" s="28" t="n">
         <v>10</v>
@@ -3108,7 +3117,7 @@
         <v>52</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D19" s="28" t="n">
         <v>1</v>
@@ -3136,7 +3145,7 @@
         <v>56</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D21" s="28" t="n">
         <v>1</v>
@@ -3150,7 +3159,7 @@
         <v>58</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D22" s="28" t="n">
         <v>9</v>
@@ -3164,7 +3173,7 @@
         <v>61</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D23" s="28" t="n">
         <v>4</v>
@@ -3178,7 +3187,7 @@
         <v>63</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D24" s="28" t="n">
         <v>9</v>
@@ -3202,7 +3211,7 @@
         <v>68</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D26" s="28" t="n">
         <v>12</v>
@@ -3216,7 +3225,7 @@
         <v>70</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D27" s="28" t="n">
         <v>13</v>
@@ -3244,7 +3253,7 @@
         <v>75</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D29" s="28" t="n">
         <v>7</v>
@@ -3258,7 +3267,7 @@
         <v>77</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D30" s="28" t="n">
         <v>15</v>
@@ -3272,7 +3281,7 @@
         <v>79</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D31" s="28" t="n">
         <v>15</v>
@@ -3296,10 +3305,10 @@
         <v>84</v>
       </c>
       <c r="C33" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="D33" s="28" t="s">
         <v>234</v>
-      </c>
-      <c r="D33" s="28" t="s">
-        <v>235</v>
       </c>
       <c r="E33" s="29" t="n">
         <v>3</v>
@@ -3310,7 +3319,7 @@
         <v>86</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D34" s="28" t="n">
         <v>16</v>
@@ -3324,7 +3333,7 @@
         <v>89</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D35" s="28" t="n">
         <v>9</v>
@@ -3338,7 +3347,7 @@
         <v>92</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D36" s="28" t="n">
         <v>4</v>
@@ -3352,7 +3361,7 @@
         <v>94</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D37" s="28" t="n">
         <v>9</v>
@@ -3366,7 +3375,7 @@
         <v>97</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D38" s="28" t="n">
         <v>9</v>
@@ -3415,10 +3424,10 @@
     </row>
     <row r="42" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D42" s="28" t="n">
         <v>8</v>
@@ -3429,10 +3438,10 @@
     </row>
     <row r="43" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D43" s="28" t="n">
         <v>15</v>
@@ -3443,10 +3452,10 @@
     </row>
     <row r="44" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D44" s="28" t="n">
         <v>15</v>
@@ -3457,23 +3466,23 @@
     </row>
     <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="35" t="s">
         <v>110</v>
-      </c>
-      <c r="C45" s="35" t="s">
-        <v>111</v>
       </c>
       <c r="D45" s="32"/>
       <c r="E45" s="33"/>
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="C46" s="27" t="s">
-        <v>113</v>
-      </c>
       <c r="D46" s="28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E46" s="29" t="n">
         <v>2</v>
@@ -3481,7 +3490,7 @@
     </row>
     <row r="47" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C47" s="35" t="s">
         <v>74</v>
@@ -3491,10 +3500,10 @@
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D48" s="28" t="n">
         <v>4</v>
@@ -3505,10 +3514,10 @@
     </row>
     <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D49" s="28" t="n">
         <v>1</v>
@@ -3519,13 +3528,13 @@
     </row>
     <row r="50" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="C50" s="27" t="s">
-        <v>120</v>
-      </c>
       <c r="D50" s="28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E50" s="29" t="n">
         <v>3</v>
@@ -3533,10 +3542,10 @@
     </row>
     <row r="51" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D51" s="28" t="n">
         <v>9</v>
@@ -3547,10 +3556,10 @@
     </row>
     <row r="52" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D52" s="28" t="n">
         <v>15</v>
@@ -3561,10 +3570,10 @@
     </row>
     <row r="53" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D53" s="28" t="n">
         <v>9</v>
@@ -3575,30 +3584,30 @@
     </row>
     <row r="54" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" s="35" t="s">
         <v>128</v>
-      </c>
-      <c r="C54" s="35" t="s">
-        <v>129</v>
       </c>
       <c r="D54" s="32"/>
       <c r="E54" s="33"/>
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" s="35" t="s">
         <v>131</v>
-      </c>
-      <c r="C55" s="35" t="s">
-        <v>132</v>
       </c>
       <c r="D55" s="32"/>
       <c r="E55" s="33"/>
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D56" s="28" t="n">
         <v>17</v>
@@ -3609,10 +3618,10 @@
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D57" s="28" t="n">
         <v>15</v>
@@ -3623,10 +3632,10 @@
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D58" s="28" t="n">
         <v>9</v>
@@ -3637,10 +3646,10 @@
     </row>
     <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C59" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D59" s="28" t="n">
         <v>9</v>
@@ -3651,13 +3660,13 @@
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="C60" s="27" t="s">
-        <v>144</v>
-      </c>
       <c r="D60" s="28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E60" s="29" t="n">
         <v>2</v>
@@ -3665,20 +3674,20 @@
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" s="35" t="s">
         <v>145</v>
-      </c>
-      <c r="C61" s="35" t="s">
-        <v>146</v>
       </c>
       <c r="D61" s="32"/>
       <c r="E61" s="33"/>
     </row>
     <row r="62" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C62" s="27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D62" s="28" t="n">
         <v>9</v>
@@ -3689,10 +3698,10 @@
     </row>
     <row r="63" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C63" s="36" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D63" s="28" t="n">
         <v>4</v>
@@ -3703,20 +3712,20 @@
     </row>
     <row r="64" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B64" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C64" s="35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D64" s="32"/>
       <c r="E64" s="33"/>
     </row>
     <row r="65" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C65" s="27" t="s">
         <v>153</v>
-      </c>
-      <c r="C65" s="27" t="s">
-        <v>154</v>
       </c>
       <c r="D65" s="28" t="n">
         <v>18</v>
@@ -3727,10 +3736,10 @@
     </row>
     <row r="66" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C66" s="27" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D66" s="28" t="n">
         <v>4</v>
@@ -3741,10 +3750,10 @@
     </row>
     <row r="67" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B67" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="27" t="s">
         <v>157</v>
-      </c>
-      <c r="C67" s="27" t="s">
-        <v>158</v>
       </c>
       <c r="D67" s="28" t="n">
         <v>1</v>
@@ -3755,10 +3764,10 @@
     </row>
     <row r="68" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C68" s="27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D68" s="28" t="n">
         <v>10</v>
@@ -3769,10 +3778,10 @@
     </row>
     <row r="69" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B69" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D69" s="28" t="n">
         <v>9</v>
@@ -3783,10 +3792,10 @@
     </row>
     <row r="70" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B70" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C70" s="27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D70" s="28" t="n">
         <v>7</v>
@@ -3797,10 +3806,10 @@
     </row>
     <row r="71" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B71" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C71" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D71" s="28" t="n">
         <v>11</v>
@@ -3811,10 +3820,10 @@
     </row>
     <row r="72" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B72" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C72" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D72" s="28" t="n">
         <v>1</v>
@@ -3825,10 +3834,10 @@
     </row>
     <row r="73" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C73" s="27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D73" s="28" t="n">
         <v>9</v>
@@ -3839,10 +3848,10 @@
     </row>
     <row r="74" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B74" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C74" s="27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D74" s="28" t="n">
         <v>4</v>
@@ -3853,10 +3862,10 @@
     </row>
     <row r="75" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B75" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C75" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D75" s="28" t="n">
         <v>15</v>
@@ -3867,10 +3876,10 @@
     </row>
     <row r="76" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C76" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D76" s="28" t="n">
         <v>15</v>
@@ -3881,10 +3890,10 @@
     </row>
     <row r="77" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C77" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D77" s="28" t="n">
         <v>15</v>
@@ -3895,10 +3904,10 @@
     </row>
     <row r="78" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C78" s="27" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D78" s="28" t="n">
         <v>4</v>
@@ -3909,30 +3918,30 @@
     </row>
     <row r="79" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B79" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="C79" s="35" t="s">
         <v>185</v>
-      </c>
-      <c r="C79" s="35" t="s">
-        <v>186</v>
       </c>
       <c r="D79" s="32"/>
       <c r="E79" s="33"/>
     </row>
     <row r="80" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B80" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="C80" s="35" t="s">
         <v>188</v>
-      </c>
-      <c r="C80" s="35" t="s">
-        <v>189</v>
       </c>
       <c r="D80" s="32"/>
       <c r="E80" s="33"/>
     </row>
     <row r="81" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B81" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C81" s="27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D81" s="28" t="n">
         <v>2</v>
@@ -3943,7 +3952,7 @@
     </row>
     <row r="82" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C82" s="27" t="s">
         <v>5</v>
@@ -3957,10 +3966,10 @@
     </row>
     <row r="83" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B83" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C83" s="27" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D83" s="28" t="n">
         <v>19</v>
@@ -3971,10 +3980,10 @@
     </row>
     <row r="84" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B84" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C84" s="27" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D84" s="28" t="n">
         <v>7</v>
@@ -3985,17 +3994,17 @@
     </row>
     <row r="85" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B85" s="34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C85" s="35" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D85" s="32"/>
       <c r="E85" s="33"/>
     </row>
     <row r="86" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B86" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C86" s="35" t="s">
         <v>42</v>
@@ -4005,10 +4014,10 @@
     </row>
     <row r="87" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B87" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C87" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D87" s="28" t="n">
         <v>15</v>
@@ -4019,10 +4028,10 @@
     </row>
     <row r="88" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B88" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C88" s="27" t="s">
         <v>205</v>
-      </c>
-      <c r="C88" s="27" t="s">
-        <v>206</v>
       </c>
       <c r="D88" s="28" t="n">
         <v>4</v>
@@ -4033,10 +4042,10 @@
     </row>
     <row r="89" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B89" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C89" s="27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D89" s="28" t="n">
         <v>2</v>
@@ -4047,7 +4056,7 @@
     </row>
     <row r="90" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B90" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C90" s="27" t="s">
         <v>55</v>
@@ -4061,10 +4070,10 @@
     </row>
     <row r="91" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B91" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C91" s="37" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D91" s="38" t="n">
         <v>4</v>
@@ -4154,74 +4163,74 @@
       <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="41" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="41" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="41" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -4250,49 +4259,49 @@
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.15"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="41" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="41" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -4304,4 +4313,578 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:C91"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.25"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="42"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="42"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="42"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="42"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="42"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="42"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="42"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="42"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="42"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="42"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="42"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="42"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="42"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="42"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="42"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="42"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="42"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="42"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="42"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="42"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="42"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="42"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="42"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="42"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="42"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="42"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="42"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="42"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="42"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="42"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="42"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="42"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="42"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="42"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="42"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="42"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="42"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="42"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="42"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="42"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="42"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="42"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="42"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="42"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" s="42"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="42"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="42"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="42"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="42"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52" s="42"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="42"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" s="42"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" s="42"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="C56" s="42"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="42"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="42"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" s="42"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="42"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" s="42"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" s="42"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63" s="42"/>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="C64" s="42"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="C65" s="42"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="44" t="s">
+        <v>155</v>
+      </c>
+      <c r="C66" s="42"/>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="42"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="C68" s="42"/>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="44" t="s">
+        <v>161</v>
+      </c>
+      <c r="C69" s="42"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C70" s="42"/>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="C71" s="42"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C72" s="42"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="C73" s="42"/>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="C74" s="42"/>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C75" s="42"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="C76" s="42"/>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="C77" s="42"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="C78" s="42"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="C79" s="42"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C80" s="42"/>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="C81" s="42"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="C82" s="42"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="C83" s="42"/>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="C84" s="42"/>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="C85" s="42"/>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="C86" s="42"/>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="44" t="s">
+        <v>202</v>
+      </c>
+      <c r="C87" s="42"/>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="44" t="s">
+        <v>204</v>
+      </c>
+      <c r="C88" s="42"/>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="C89" s="42"/>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="44" t="s">
+        <v>208</v>
+      </c>
+      <c r="C90" s="42"/>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="C91" s="42"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>